<commit_message>
Remove deprecated app_refactored.py file and update README to include OLA Maps API Testing features. Added new requirements for HTTP requests and updated session state management in app.py. Enhanced analytics dashboard rendering for better layout. Updated commands documentation for running the application.
</commit_message>
<xml_diff>
--- a/utils/places.xlsx
+++ b/utils/places.xlsx
@@ -498,50 +498,50 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>51.5074</v>
+        <v>48.8584</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1278</v>
+        <v>2.2945</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The Ritz London</t>
+          <t>Eiffel Tower</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>150 Piccadilly, St. James's, London</t>
+          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>123457</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45897.90878924612</v>
+        <v>45897.90879825589</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>45898.08307190106</v>
+        <v>45897.90879825589</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>35.6762</v>
+        <v>40.7128</v>
       </c>
       <c r="C3" t="n">
-        <v>139.6503</v>
+        <v>-74.006</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -550,183 +550,183 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Tokyo Tower</t>
+          <t>Statue of Liberty</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
+          <t>Liberty Island, New York, NY</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>105-0011</t>
+          <t>10004</t>
         </is>
       </c>
       <c r="H3" s="2" t="n">
-        <v>45897.90879374704</v>
+        <v>45897.90915786968</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>45897.90879374704</v>
+        <v>45897.90915786968</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>48.8584</v>
+        <v>34.0522</v>
       </c>
       <c r="C4" t="n">
-        <v>2.2945</v>
+        <v>-118.2437</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Eiffel Tower</t>
+          <t>In-N-Out Burger</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
+          <t>7000 Sunset Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>90028</t>
         </is>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45897.90879825589</v>
+        <v>45897.90916285996</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>45897.90879825589</v>
+        <v>45897.90916285996</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>40.7128</v>
+        <v>51.5074</v>
       </c>
       <c r="C5" t="n">
-        <v>-74.006</v>
+        <v>-0.1278</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Statue of Liberty</t>
+          <t>The Ritz London</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Liberty Island, New York, NY</t>
+          <t>150 Piccadilly, St. James's, London</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>10004</t>
+          <t>W1J 9BR</t>
         </is>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45897.90915786968</v>
+        <v>45897.90916762971</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>45897.90915786968</v>
+        <v>45897.90916762971</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>34.0522</v>
+        <v>35.6762</v>
       </c>
       <c r="C6" t="n">
-        <v>-118.2437</v>
+        <v>139.6503</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>In-N-Out Burger</t>
+          <t>Tokyo Tower</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>7000 Sunset Blvd, Los Angeles, CA</t>
+          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>90028</t>
+          <t>105-0011</t>
         </is>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45897.90916285996</v>
+        <v>45897.90917233432</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>45897.90916285996</v>
+        <v>45897.90917233432</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>51.5074</v>
+        <v>48.8584</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1278</v>
+        <v>2.2945</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>The Ritz London</t>
+          <t>Eiffel Tower</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>150 Piccadilly, St. James's, London</t>
+          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>W1J 9BR</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45897.90916762971</v>
+        <v>45897.9091771625</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>45897.90916762971</v>
+        <v>45897.9091771625</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>35.6762</v>
+        <v>40.7128</v>
       </c>
       <c r="C8" t="n">
-        <v>139.6503</v>
+        <v>-74.006</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -735,183 +735,183 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Tokyo Tower</t>
+          <t>Statue of Liberty</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
+          <t>Liberty Island, New York, NY</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>105-0011</t>
+          <t>10004</t>
         </is>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45897.90917233432</v>
+        <v>45897.91335162918</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>45897.90917233432</v>
+        <v>45897.91335162918</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>48.8584</v>
+        <v>34.0522</v>
       </c>
       <c r="C9" t="n">
-        <v>2.2945</v>
+        <v>-118.2437</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Eiffel Tower</t>
+          <t>In-N-Out Burger</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
+          <t>7000 Sunset Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>90028</t>
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45897.9091771625</v>
+        <v>45897.91335396986</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>45897.9091771625</v>
+        <v>45897.91335396986</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>40.7128</v>
+        <v>51.5074</v>
       </c>
       <c r="C10" t="n">
-        <v>-74.006</v>
+        <v>-0.1278</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Statue of Liberty</t>
+          <t>The Ritz London</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Liberty Island, New York, NY</t>
+          <t>150 Piccadilly, St. James's, London</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>10004</t>
+          <t>W1J 9BR</t>
         </is>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45897.91335162918</v>
+        <v>45897.9133557985</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>45897.91335162918</v>
+        <v>45897.9133557985</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>34.0522</v>
+        <v>35.6762</v>
       </c>
       <c r="C11" t="n">
-        <v>-118.2437</v>
+        <v>139.6503</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>In-N-Out Burger</t>
+          <t>Tokyo Tower</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>7000 Sunset Blvd, Los Angeles, CA</t>
+          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>90028</t>
+          <t>105-0011</t>
         </is>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45897.91335396986</v>
+        <v>45897.91335730844</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>45897.91335396986</v>
+        <v>45897.91335730844</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>51.5074</v>
+        <v>48.8584</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.1278</v>
+        <v>2.2945</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>The Ritz London</t>
+          <t>Eiffel Tower</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>150 Piccadilly, St. James's, London</t>
+          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>W1J 9BR</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H12" s="2" t="n">
-        <v>45897.9133557985</v>
+        <v>45897.91335884258</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>45897.9133557985</v>
+        <v>45897.91335884258</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>35.6762</v>
+        <v>40.7128</v>
       </c>
       <c r="C13" t="n">
-        <v>139.6503</v>
+        <v>-74.006</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -920,183 +920,183 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Tokyo Tower</t>
+          <t>Statue of Liberty</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
+          <t>Liberty Island, New York, NY</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>105-0011</t>
+          <t>10004</t>
         </is>
       </c>
       <c r="H13" s="2" t="n">
-        <v>45897.91335730844</v>
+        <v>45897.9138873342</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>45897.91335730844</v>
+        <v>45897.9138873342</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>48.8584</v>
+        <v>34.0522</v>
       </c>
       <c r="C14" t="n">
-        <v>2.2945</v>
+        <v>-118.2437</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Eiffel Tower</t>
+          <t>In-N-Out Burger</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
+          <t>7000 Sunset Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>90028</t>
         </is>
       </c>
       <c r="H14" s="2" t="n">
-        <v>45897.91335884258</v>
+        <v>45897.91388881483</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>45897.91335884258</v>
+        <v>45897.91388881483</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>40.7128</v>
+        <v>51.5074</v>
       </c>
       <c r="C15" t="n">
-        <v>-74.006</v>
+        <v>-0.1278</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Statue of Liberty</t>
+          <t>The Ritz London</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Liberty Island, New York, NY</t>
+          <t>150 Piccadilly, St. James's, London</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>10004</t>
+          <t>W1J 9BR</t>
         </is>
       </c>
       <c r="H15" s="2" t="n">
-        <v>45897.9138873342</v>
+        <v>45897.91389030834</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>45897.9138873342</v>
+        <v>45897.91389030834</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>34.0522</v>
+        <v>35.6762</v>
       </c>
       <c r="C16" t="n">
-        <v>-118.2437</v>
+        <v>139.6503</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>In-N-Out Burger</t>
+          <t>Tokyo Tower</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>7000 Sunset Blvd, Los Angeles, CA</t>
+          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>90028</t>
+          <t>105-0011</t>
         </is>
       </c>
       <c r="H16" s="2" t="n">
-        <v>45897.91388881483</v>
+        <v>45897.91389178917</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>45897.91388881483</v>
+        <v>45897.91389178917</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>51.5074</v>
+        <v>48.8584</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.1278</v>
+        <v>2.2945</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>The Ritz London</t>
+          <t>Eiffel Tower</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>150 Piccadilly, St. James's, London</t>
+          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>W1J 9BR</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H17" s="2" t="n">
-        <v>45897.91389030834</v>
+        <v>45897.91389325335</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>45897.91389030834</v>
+        <v>45897.91389325335</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>35.6762</v>
+        <v>40.7128</v>
       </c>
       <c r="C18" t="n">
-        <v>139.6503</v>
+        <v>-74.006</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1105,442 +1105,442 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Tokyo Tower</t>
+          <t>Statue of Liberty</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
+          <t>Liberty Island, New York, NY</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>105-0011</t>
+          <t>10004</t>
         </is>
       </c>
       <c r="H18" s="2" t="n">
-        <v>45897.91389178917</v>
+        <v>45897.91439854987</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>45897.91389178917</v>
+        <v>45897.91439854987</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>48.8584</v>
+        <v>34.0522</v>
       </c>
       <c r="C19" t="n">
-        <v>2.2945</v>
+        <v>-118.2437</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Eiffel Tower</t>
+          <t>In-N-Out Burger</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
+          <t>7000 Sunset Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>90028</t>
         </is>
       </c>
       <c r="H19" s="2" t="n">
-        <v>45897.91389325335</v>
+        <v>45897.91440005886</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>45897.91389325335</v>
+        <v>45897.91440005886</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>40.7128</v>
+        <v>51.5074</v>
       </c>
       <c r="C20" t="n">
-        <v>-74.006</v>
+        <v>-0.1278</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Statue of Liberty</t>
+          <t>The Ritz London</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Liberty Island, New York, NY</t>
+          <t>150 Piccadilly, St. James's, London</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>10004</t>
+          <t>W1J 9BR</t>
         </is>
       </c>
       <c r="H20" s="2" t="n">
-        <v>45897.91439854987</v>
+        <v>45897.91440155123</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>45897.91439854987</v>
+        <v>45897.91440155123</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>34.0522</v>
+        <v>35.6762</v>
       </c>
       <c r="C21" t="n">
-        <v>-118.2437</v>
+        <v>139.6503</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>In-N-Out Burger</t>
+          <t>Tokyo Tower</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>7000 Sunset Blvd, Los Angeles, CA</t>
+          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>90028</t>
+          <t>105-0011</t>
         </is>
       </c>
       <c r="H21" s="2" t="n">
-        <v>45897.91440005886</v>
+        <v>45897.9144030321</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>45897.91440005886</v>
+        <v>45897.9144030321</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>51.5074</v>
+        <v>48.8584</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.1278</v>
+        <v>2.2945</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>The Ritz London</t>
+          <t>Eiffel Tower</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>150 Piccadilly, St. James's, London</t>
+          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>W1J 9BR</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H22" s="2" t="n">
-        <v>45897.91440155123</v>
+        <v>45897.91440450991</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>45897.91440155123</v>
+        <v>45897.91440450991</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>35.6762</v>
+        <v>3.2800025</v>
       </c>
       <c r="C23" t="n">
-        <v>139.6503</v>
+        <v>70.00000199999999</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>dfhsdfhdfshdsfh</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Tokyo Tower</t>
+          <t>12.993103152916301,77.54332622119354</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
+          <t>13/23 Edison Road B-Zone Durgapur-5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>105-0011</t>
+          <t>713205</t>
         </is>
       </c>
       <c r="H23" s="2" t="n">
-        <v>45897.9144030321</v>
+        <v>45897.91544395484</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>45897.9144030321</v>
+        <v>45897.91544395484</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>48.8584</v>
+        <v>3.2800025</v>
       </c>
       <c r="C24" t="n">
-        <v>2.2945</v>
+        <v>70.00000199999999</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>dfhsdfhdfshdsfh</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Eiffel Tower</t>
+          <t>12.993103152916301,77.54332622119354</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
+          <t>13/23 Edison Road B-Zone Durgapur-5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>713205</t>
         </is>
       </c>
       <c r="H24" s="2" t="n">
-        <v>45897.91440450991</v>
+        <v>45897.91552547592</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>45897.91440450991</v>
+        <v>45897.91552547592</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>3.2800025</v>
+        <v>40.7128</v>
       </c>
       <c r="C25" t="n">
-        <v>70.00000199999999</v>
+        <v>-74.006</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>dfhsdfhdfshdsfh</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>12.993103152916301,77.54332622119354</t>
+          <t>Statue of Liberty</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>13/23 Edison Road B-Zone Durgapur-5</t>
+          <t>Liberty Island, New York, NY</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>713205</t>
+          <t>10004</t>
         </is>
       </c>
       <c r="H25" s="2" t="n">
-        <v>45897.91544395484</v>
+        <v>45897.93610299593</v>
       </c>
       <c r="I25" s="2" t="n">
-        <v>45897.91544395484</v>
+        <v>45897.93610299593</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>3.2800025</v>
+        <v>34.0522</v>
       </c>
       <c r="C26" t="n">
-        <v>70.00000199999999</v>
+        <v>-118.2437</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>dfhsdfhdfshdsfh</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>12.993103152916301,77.54332622119354</t>
+          <t>In-N-Out Burger</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>13/23 Edison Road B-Zone Durgapur-5</t>
+          <t>7000 Sunset Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>713205</t>
+          <t>90028</t>
         </is>
       </c>
       <c r="H26" s="2" t="n">
-        <v>45897.91552547592</v>
+        <v>45897.9361051696</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>45897.91552547592</v>
+        <v>45897.9361051696</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>40.7128</v>
+        <v>51.5074</v>
       </c>
       <c r="C27" t="n">
-        <v>-74.006</v>
+        <v>-0.1278</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Statue of Liberty</t>
+          <t>The Ritz London</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Liberty Island, New York, NY</t>
+          <t>150 Piccadilly, St. James's, London</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>10004</t>
+          <t>W1J 9BR</t>
         </is>
       </c>
       <c r="H27" s="2" t="n">
-        <v>45897.93610299593</v>
+        <v>45897.93610670909</v>
       </c>
       <c r="I27" s="2" t="n">
-        <v>45897.93610299593</v>
+        <v>45897.93610670909</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>34.0522</v>
+        <v>35.6762</v>
       </c>
       <c r="C28" t="n">
-        <v>-118.2437</v>
+        <v>139.6503</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>In-N-Out Burger</t>
+          <t>Tokyo Tower</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>7000 Sunset Blvd, Los Angeles, CA</t>
+          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>90028</t>
+          <t>105-0011</t>
         </is>
       </c>
       <c r="H28" s="2" t="n">
-        <v>45897.9361051696</v>
+        <v>45897.93610820181</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>45897.9361051696</v>
+        <v>45897.93610820181</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>51.5074</v>
+        <v>48.8584</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.1278</v>
+        <v>2.2945</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>The Ritz London</t>
+          <t>Eiffel Tower</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>150 Piccadilly, St. James's, London</t>
+          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>W1J 9BR</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H29" s="2" t="n">
-        <v>45897.93610670909</v>
+        <v>45897.93610970074</v>
       </c>
       <c r="I29" s="2" t="n">
-        <v>45897.93610670909</v>
+        <v>45897.93610970074</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>35.6762</v>
+        <v>40.7589</v>
       </c>
       <c r="C30" t="n">
-        <v>139.6503</v>
+        <v>-73.9851</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1549,109 +1549,109 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Tokyo Tower</t>
+          <t>Times Square</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
+          <t>Manhattan, New York, NY</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>105-0011</t>
+          <t>10036</t>
         </is>
       </c>
       <c r="H30" s="2" t="n">
-        <v>45897.93610820181</v>
+        <v>45897.93611120526</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>45897.93610820181</v>
+        <v>45897.93611120526</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>48.8584</v>
+        <v>34.1016</v>
       </c>
       <c r="C31" t="n">
-        <v>2.2945</v>
+        <v>-118.3267</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Eiffel Tower</t>
+          <t>The Ivy</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
+          <t>113 N Robertson Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>90048</t>
         </is>
       </c>
       <c r="H31" s="2" t="n">
-        <v>45897.93610970074</v>
+        <v>45897.93611271458</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>45897.93610970074</v>
+        <v>45897.93611271458</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>40.7589</v>
+        <v>51.5007</v>
       </c>
       <c r="C32" t="n">
-        <v>-73.9851</v>
+        <v>-0.1246</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Times Square</t>
+          <t>The Savoy</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Manhattan, New York, NY</t>
+          <t>Strand, London</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>10036</t>
+          <t>WC2R 0EZ</t>
         </is>
       </c>
       <c r="H32" s="2" t="n">
-        <v>45897.93611120526</v>
+        <v>45897.93611421469</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>45897.93611120526</v>
+        <v>45897.93611421469</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B33" t="n">
-        <v>34.1016</v>
+        <v>35.6586</v>
       </c>
       <c r="C33" t="n">
-        <v>-118.3267</v>
+        <v>139.7454</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1660,35 +1660,35 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>The Ivy</t>
+          <t>Sukiyabashi Jiro</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>113 N Robertson Blvd, Los Angeles, CA</t>
+          <t>4-2-15 Ginza, Chuo City, Tokyo</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>90048</t>
+          <t>104-0061</t>
         </is>
       </c>
       <c r="H33" s="2" t="n">
-        <v>45897.93611271458</v>
+        <v>45897.936115736</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>45897.93611271458</v>
+        <v>45897.936115736</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B34" t="n">
-        <v>51.5007</v>
+        <v>48.8738</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.1246</v>
+        <v>2.295</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1697,35 +1697,35 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>The Savoy</t>
+          <t>Hotel Ritz Paris</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Strand, London</t>
+          <t>15 Place Vendôme, Paris</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>WC2R 0EZ</t>
+          <t>75001</t>
         </is>
       </c>
       <c r="H34" s="2" t="n">
-        <v>45897.93611421469</v>
+        <v>45897.93611725241</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>45897.93611421469</v>
+        <v>45897.93611725241</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B35" t="n">
-        <v>35.6586</v>
+        <v>40.7484</v>
       </c>
       <c r="C35" t="n">
-        <v>139.7454</v>
+        <v>-73.98569999999999</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1734,35 +1734,35 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Sukiyabashi Jiro</t>
+          <t>Le Bernardin</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>4-2-15 Ginza, Chuo City, Tokyo</t>
+          <t>155 W 51st St, New York, NY</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>104-0061</t>
+          <t>10019</t>
         </is>
       </c>
       <c r="H35" s="2" t="n">
-        <v>45897.936115736</v>
+        <v>45897.93611875152</v>
       </c>
       <c r="I35" s="2" t="n">
-        <v>45897.936115736</v>
+        <v>45897.93611875152</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B36" t="n">
-        <v>48.8738</v>
+        <v>34.0736</v>
       </c>
       <c r="C36" t="n">
-        <v>2.295</v>
+        <v>-118.24</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1771,109 +1771,109 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Hotel Ritz Paris</t>
+          <t>Beverly Hills Hotel</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>15 Place Vendôme, Paris</t>
+          <t>9641 Sunset Blvd, Beverly Hills, CA</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>75001</t>
+          <t>90210</t>
         </is>
       </c>
       <c r="H36" s="2" t="n">
-        <v>45897.93611725241</v>
+        <v>45897.93612025098</v>
       </c>
       <c r="I36" s="2" t="n">
-        <v>45897.93611725241</v>
+        <v>45897.93612025098</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B37" t="n">
-        <v>40.7484</v>
+        <v>51.5194</v>
       </c>
       <c r="C37" t="n">
-        <v>-73.98569999999999</v>
+        <v>-0.127</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Le Bernardin</t>
+          <t>Big Ben</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>155 W 51st St, New York, NY</t>
+          <t>Westminster, London</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>10019</t>
+          <t>SW1A 0AA</t>
         </is>
       </c>
       <c r="H37" s="2" t="n">
-        <v>45897.93611875152</v>
+        <v>45897.93612173742</v>
       </c>
       <c r="I37" s="2" t="n">
-        <v>45897.93611875152</v>
+        <v>45897.93612173742</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B38" t="n">
-        <v>34.0736</v>
+        <v>35.6895</v>
       </c>
       <c r="C38" t="n">
-        <v>-118.24</v>
+        <v>139.6917</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Beverly Hills Hotel</t>
+          <t>Narisawa</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>9641 Sunset Blvd, Beverly Hills, CA</t>
+          <t>2-6-15 Minato, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>90210</t>
+          <t>107-0062</t>
         </is>
       </c>
       <c r="H38" s="2" t="n">
-        <v>45897.93612025098</v>
+        <v>45897.93612323149</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>45897.93612025098</v>
+        <v>45897.93612323149</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B39" t="n">
-        <v>51.5194</v>
+        <v>48.8606</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.127</v>
+        <v>2.3376</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1882,72 +1882,72 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Big Ben</t>
+          <t>Louvre Museum</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Westminster, London</t>
+          <t>Rue de Rivoli, Paris</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>SW1A 0AA</t>
+          <t>75001</t>
         </is>
       </c>
       <c r="H39" s="2" t="n">
-        <v>45897.93612173742</v>
+        <v>45897.93612472359</v>
       </c>
       <c r="I39" s="2" t="n">
-        <v>45897.93612173742</v>
+        <v>45897.93612472359</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B40" t="n">
-        <v>35.6895</v>
+        <v>40.7505</v>
       </c>
       <c r="C40" t="n">
-        <v>139.6917</v>
+        <v>-73.99339999999999</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Narisawa</t>
+          <t>The Plaza</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2-6-15 Minato, Minato City, Tokyo</t>
+          <t>768 5th Ave, New York, NY</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>107-0062</t>
+          <t>10019</t>
         </is>
       </c>
       <c r="H40" s="2" t="n">
-        <v>45897.93612323149</v>
+        <v>45897.93612623157</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>45897.93612323149</v>
+        <v>45897.93612623157</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B41" t="n">
-        <v>48.8606</v>
+        <v>34.0928</v>
       </c>
       <c r="C41" t="n">
-        <v>2.3376</v>
+        <v>-118.3287</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1956,109 +1956,109 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Louvre Museum</t>
+          <t>Hollywood Walk of Fame</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Rue de Rivoli, Paris</t>
+          <t>Hollywood Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>75001</t>
+          <t>90028</t>
         </is>
       </c>
       <c r="H41" s="2" t="n">
-        <v>45897.93612472359</v>
+        <v>45897.93612772214</v>
       </c>
       <c r="I41" s="2" t="n">
-        <v>45897.93612472359</v>
+        <v>45897.93612772214</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B42" t="n">
-        <v>40.7505</v>
+        <v>51.5033</v>
       </c>
       <c r="C42" t="n">
-        <v>-73.99339999999999</v>
+        <v>-0.1195</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>The Plaza</t>
+          <t>Gordon Ramsay Restaurant</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>768 5th Ave, New York, NY</t>
+          <t>68 Royal Hospital Rd, London</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>10019</t>
+          <t>SW3 4HP</t>
         </is>
       </c>
       <c r="H42" s="2" t="n">
-        <v>45897.93612623157</v>
+        <v>45897.9361292375</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>45897.93612623157</v>
+        <v>45897.9361292375</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B43" t="n">
-        <v>34.0928</v>
+        <v>35.6812</v>
       </c>
       <c r="C43" t="n">
-        <v>-118.3287</v>
+        <v>139.7671</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Hollywood Walk of Fame</t>
+          <t>Park Hyatt Tokyo</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Hollywood Blvd, Los Angeles, CA</t>
+          <t>3-7-1-2 Nishi-Shinjuku, Tokyo</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>90028</t>
+          <t>163-1055</t>
         </is>
       </c>
       <c r="H43" s="2" t="n">
-        <v>45897.93612772214</v>
+        <v>45897.93613075427</v>
       </c>
       <c r="I43" s="2" t="n">
-        <v>45897.93612772214</v>
+        <v>45897.93613075427</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B44" t="n">
-        <v>51.5033</v>
+        <v>48.8589</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.1195</v>
+        <v>2.32</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -2067,146 +2067,146 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Gordon Ramsay Restaurant</t>
+          <t>L'Arpège</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>68 Royal Hospital Rd, London</t>
+          <t>84 Rue de Varenne, Paris</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>SW3 4HP</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H44" s="2" t="n">
-        <v>45897.9361292375</v>
+        <v>45897.93613226698</v>
       </c>
       <c r="I44" s="2" t="n">
-        <v>45897.9361292375</v>
+        <v>45897.93613226698</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B45" t="n">
-        <v>35.6812</v>
+        <v>40.7587</v>
       </c>
       <c r="C45" t="n">
-        <v>139.7671</v>
+        <v>-73.9787</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Park Hyatt Tokyo</t>
+          <t>Per Se</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>3-7-1-2 Nishi-Shinjuku, Tokyo</t>
+          <t>10 Columbus Circle, New York, NY</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>163-1055</t>
+          <t>10019</t>
         </is>
       </c>
       <c r="H45" s="2" t="n">
-        <v>45897.93613075427</v>
+        <v>45897.93613376309</v>
       </c>
       <c r="I45" s="2" t="n">
-        <v>45897.93613075427</v>
+        <v>45897.93613376309</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B46" t="n">
-        <v>48.8589</v>
+        <v>34.0522</v>
       </c>
       <c r="C46" t="n">
-        <v>2.32</v>
+        <v>-118.2437</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>L'Arpège</t>
+          <t>The Beverly Hills Hotel</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>84 Rue de Varenne, Paris</t>
+          <t>9641 Sunset Blvd, Beverly Hills, CA</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>90210</t>
         </is>
       </c>
       <c r="H46" s="2" t="n">
-        <v>45897.93613226698</v>
+        <v>45897.93613527065</v>
       </c>
       <c r="I46" s="2" t="n">
-        <v>45897.93613226698</v>
+        <v>45897.93613527065</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B47" t="n">
-        <v>40.7587</v>
+        <v>51.5074</v>
       </c>
       <c r="C47" t="n">
-        <v>-73.9787</v>
+        <v>-0.1278</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Per Se</t>
+          <t>Buckingham Palace</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>10 Columbus Circle, New York, NY</t>
+          <t>London</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>10019</t>
+          <t>SW1A 1AA</t>
         </is>
       </c>
       <c r="H47" s="2" t="n">
-        <v>45897.93613376309</v>
+        <v>45897.93613682182</v>
       </c>
       <c r="I47" s="2" t="n">
-        <v>45897.93613376309</v>
+        <v>45897.93613682182</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B48" t="n">
-        <v>34.0522</v>
+        <v>35.6762</v>
       </c>
       <c r="C48" t="n">
-        <v>-118.2437</v>
+        <v>139.6503</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -2215,146 +2215,146 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>The Beverly Hills Hotel</t>
+          <t>Aman Tokyo</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>9641 Sunset Blvd, Beverly Hills, CA</t>
+          <t>1-5-6 Otemachi, Tokyo</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>90210</t>
+          <t>100-0004</t>
         </is>
       </c>
       <c r="H48" s="2" t="n">
-        <v>45897.93613527065</v>
+        <v>45897.93613834404</v>
       </c>
       <c r="I48" s="2" t="n">
-        <v>45897.93613527065</v>
+        <v>45897.93613834404</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B49" t="n">
-        <v>51.5074</v>
+        <v>48.8566</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.1278</v>
+        <v>2.3522</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Buckingham Palace</t>
+          <t>Four Seasons Hotel George V</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>31 Avenue George V, Paris</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>SW1A 1AA</t>
+          <t>75008</t>
         </is>
       </c>
       <c r="H49" s="2" t="n">
-        <v>45897.93613682182</v>
+        <v>45897.93613983144</v>
       </c>
       <c r="I49" s="2" t="n">
-        <v>45897.93613682182</v>
+        <v>45897.93613983144</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B50" t="n">
-        <v>35.6762</v>
+        <v>40.7829</v>
       </c>
       <c r="C50" t="n">
-        <v>139.6503</v>
+        <v>-73.9654</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Aman Tokyo</t>
+          <t>Eleven Madison Park</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1-5-6 Otemachi, Tokyo</t>
+          <t>11 Madison Ave, New York, NY</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>100-0004</t>
+          <t>10010</t>
         </is>
       </c>
       <c r="H50" s="2" t="n">
-        <v>45897.93613834404</v>
+        <v>45897.93614133019</v>
       </c>
       <c r="I50" s="2" t="n">
-        <v>45897.93613834404</v>
+        <v>45897.93614133019</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B51" t="n">
-        <v>48.8566</v>
+        <v>34.0736</v>
       </c>
       <c r="C51" t="n">
-        <v>2.3522</v>
+        <v>-118.24</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Four Seasons Hotel George V</t>
+          <t>Rodeo Drive</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>31 Avenue George V, Paris</t>
+          <t>Beverly Hills, CA</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>75008</t>
+          <t>90210</t>
         </is>
       </c>
       <c r="H51" s="2" t="n">
-        <v>45897.93613983144</v>
+        <v>45897.93614283481</v>
       </c>
       <c r="I51" s="2" t="n">
-        <v>45897.93613983144</v>
+        <v>45897.93614283481</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B52" t="n">
-        <v>40.7829</v>
+        <v>51.4994</v>
       </c>
       <c r="C52" t="n">
-        <v>-73.9654</v>
+        <v>-0.1245</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -2363,35 +2363,35 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Eleven Madison Park</t>
+          <t>Sketch</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>11 Madison Ave, New York, NY</t>
+          <t>9 Conduit St, London</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>10010</t>
+          <t>W1S 2XG</t>
         </is>
       </c>
       <c r="H52" s="2" t="n">
-        <v>45897.93614133019</v>
+        <v>45897.93614432773</v>
       </c>
       <c r="I52" s="2" t="n">
-        <v>45897.93614133019</v>
+        <v>45897.93614432773</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B53" t="n">
-        <v>34.0736</v>
+        <v>35.6895</v>
       </c>
       <c r="C53" t="n">
-        <v>-118.24</v>
+        <v>139.6917</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -2400,35 +2400,35 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Rodeo Drive</t>
+          <t>Shibuya Crossing</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Beverly Hills, CA</t>
+          <t>Shibuya City, Tokyo</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>90210</t>
+          <t>150-0002</t>
         </is>
       </c>
       <c r="H53" s="2" t="n">
-        <v>45897.93614283481</v>
+        <v>45897.93614582055</v>
       </c>
       <c r="I53" s="2" t="n">
-        <v>45897.93614283481</v>
+        <v>45897.93614582055</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B54" t="n">
-        <v>51.4994</v>
+        <v>48.8584</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.1245</v>
+        <v>2.2945</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -2437,165 +2437,165 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Sketch</t>
+          <t>L'Astrance</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>9 Conduit St, London</t>
+          <t>4 Rue Beethoven, Paris</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>W1S 2XG</t>
+          <t>75016</t>
         </is>
       </c>
       <c r="H54" s="2" t="n">
-        <v>45897.93614432773</v>
+        <v>45897.93614730847</v>
       </c>
       <c r="I54" s="2" t="n">
-        <v>45897.93614432773</v>
+        <v>45897.93614730847</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B55" t="n">
-        <v>35.6895</v>
+        <v>20</v>
       </c>
       <c r="C55" t="n">
-        <v>139.6917</v>
+        <v>40</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>Untitledvzxc</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Shibuya Crossing</t>
+          <t>restaurant, cafe</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Shibuya City, Tokyo</t>
+          <t>13/23 Edison Road B-Zone Durgapur-5</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>150-0002</t>
+          <t>713205</t>
         </is>
       </c>
       <c r="H55" s="2" t="n">
-        <v>45897.93614582055</v>
+        <v>45897.93933683654</v>
       </c>
       <c r="I55" s="2" t="n">
-        <v>45897.93614582055</v>
+        <v>45897.93933683654</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B56" t="n">
-        <v>48.8584</v>
+        <v>40.7128</v>
       </c>
       <c r="C56" t="n">
-        <v>2.2945</v>
+        <v>-74.006</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>L'Astrance</t>
+          <t>Statue of Liberty</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>4 Rue Beethoven, Paris</t>
+          <t>Liberty Island, New York, NY</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>75016</t>
+          <t>10004</t>
         </is>
       </c>
       <c r="H56" s="2" t="n">
-        <v>45897.93614730847</v>
+        <v>45897.94695457577</v>
       </c>
       <c r="I56" s="2" t="n">
-        <v>45897.93614730847</v>
+        <v>45897.94695457577</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B57" t="n">
-        <v>20</v>
+        <v>34.0522</v>
       </c>
       <c r="C57" t="n">
-        <v>40</v>
+        <v>-118.2437</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Untitledvzxc</t>
+          <t>restaurant</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>restaurant, cafe</t>
+          <t>In-N-Out Burger</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>13/23 Edison Road B-Zone Durgapur-5</t>
+          <t>7000 Sunset Blvd, Los Angeles, CA</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>713205</t>
+          <t>90028</t>
         </is>
       </c>
       <c r="H57" s="2" t="n">
-        <v>45897.93933683654</v>
+        <v>45897.94695457577</v>
       </c>
       <c r="I57" s="2" t="n">
-        <v>45897.93933683654</v>
+        <v>45897.94695457577</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B58" t="n">
-        <v>40.7128</v>
+        <v>51.5074</v>
       </c>
       <c r="C58" t="n">
-        <v>-74.006</v>
+        <v>-0.1278</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Statue of Liberty</t>
+          <t>The Ritz London</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Liberty Island, New York, NY</t>
+          <t>150 Piccadilly, St. James's, London</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>10004</t>
+          <t>W1J 9BR</t>
         </is>
       </c>
       <c r="H58" s="2" t="n">
@@ -2607,32 +2607,32 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B59" t="n">
-        <v>34.0522</v>
+        <v>35.6762</v>
       </c>
       <c r="C59" t="n">
-        <v>-118.2437</v>
+        <v>139.6503</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>In-N-Out Burger</t>
+          <t>Tokyo Tower</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>7000 Sunset Blvd, Los Angeles, CA</t>
+          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>90028</t>
+          <t>105-0011</t>
         </is>
       </c>
       <c r="H59" s="2" t="n">
@@ -2644,32 +2644,32 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B60" t="n">
-        <v>51.5074</v>
+        <v>48.8584</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.1278</v>
+        <v>2.2945</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>hotel</t>
+          <t>tourist_attraction</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>The Ritz London</t>
+          <t>Eiffel Tower</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>150 Piccadilly, St. James's, London</t>
+          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>W1J 9BR</t>
+          <t>75007</t>
         </is>
       </c>
       <c r="H60" s="2" t="n">
@@ -2681,50 +2681,50 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="B61" t="n">
-        <v>35.6762</v>
+        <v>51.5074</v>
       </c>
       <c r="C61" t="n">
-        <v>139.6503</v>
+        <v>-0.1278</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>tourist_attraction</t>
+          <t>hotel</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Tokyo Tower</t>
+          <t>The Ritz London</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
+          <t>150 Piccadilly, St. James's, London</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>105-0011</t>
+          <t>123457</t>
         </is>
       </c>
       <c r="H61" s="2" t="n">
-        <v>45897.94695457577</v>
+        <v>45897.90878924612</v>
       </c>
       <c r="I61" s="2" t="n">
-        <v>45897.94695457577</v>
+        <v>45898.08307190106</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="B62" t="n">
-        <v>48.8584</v>
+        <v>35.6762</v>
       </c>
       <c r="C62" t="n">
-        <v>2.2945</v>
+        <v>139.6503</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -2733,24 +2733,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Eiffel Tower</t>
+          <t>Tokyo Tower</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Champ de Mars, 5 Avenue Anatole France, Paris</t>
+          <t>4 Chome-2-8 Shibakoen, Minato City, Tokyo</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>75007</t>
+          <t>105-0011</t>
         </is>
       </c>
       <c r="H62" s="2" t="n">
-        <v>45897.94695457577</v>
+        <v>45897.90879374704</v>
       </c>
       <c r="I62" s="2" t="n">
-        <v>45897.94695457577</v>
+        <v>45897.90879374704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>